<commit_message>
addded 6 lab and reworked 5
</commit_message>
<xml_diff>
--- a/Книга1.xlsx
+++ b/Книга1.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -190,7 +191,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -596,22 +596,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>329</c:v>
+                  <c:v>343</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>171</c:v>
+                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>180</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>183</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>187</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3979,8 +3979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4037,22 +4037,22 @@
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:7" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="C4" s="2">
-        <v>171</v>
+        <v>234</v>
       </c>
       <c r="D4" s="2">
-        <v>180</v>
+        <v>250</v>
       </c>
       <c r="E4" s="2">
-        <v>180</v>
+        <v>250</v>
       </c>
       <c r="F4" s="2">
-        <v>183</v>
+        <v>250</v>
       </c>
       <c r="G4" s="2">
-        <v>187</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>

</xml_diff>